<commit_message>
1. Update Import Person can add automatically to database. 2. Update database tabel terkait RBAC karena salah koma doang.. gila nggak tuh 3. Template Upload Employee protect with password 1 and chek validate template
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/general/employee_upload.xlsx
+++ b/file/template/pusdiklat/general/employee_upload.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>BPPK</t>
   </si>
@@ -271,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,23 +307,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,6 +326,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -356,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -383,43 +390,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -530,12 +500,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,24 +533,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,76 +555,92 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -944,7 +947,7 @@
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,1333 +960,1336 @@
     <col min="6" max="6" width="5" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="10" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="J1" s="16" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="J1" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="12"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
+      <c r="A4" s="26">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="18">
         <v>4</v>
       </c>
-      <c r="E4" s="25" t="str">
+      <c r="E4" s="19" t="str">
         <f>VLOOKUP(D4,J23:K26,2)</f>
         <v>PRANATA KOMPUTER</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="21">
         <v>389</v>
       </c>
-      <c r="G4" s="26" t="str">
+      <c r="G4" s="20" t="str">
         <f>VLOOKUP(F4,J4:L19,2)</f>
         <v>1213010100</v>
       </c>
-      <c r="H4" s="26" t="str">
+      <c r="H4" s="20" t="str">
         <f>VLOOKUP(F4,J4:L19,3)</f>
         <v>Subbagian Tata Usaha, Kepegawaian Dan Hubungan Mas...</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>387</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="A5" s="26">
         <v>2</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="25" t="e">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="19" t="e">
         <f t="shared" ref="E5:E43" si="0">VLOOKUP(D5,J24:K27,2)</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26" t="e">
+      <c r="F5" s="21"/>
+      <c r="G5" s="20" t="e">
         <f t="shared" ref="G5:G42" si="1">VLOOKUP(F5,J5:L20,2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="26" t="e">
+      <c r="H5" s="20" t="e">
         <f t="shared" ref="H5:H43" si="2">VLOOKUP(F5,J5:L20,3)</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>388</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="26">
         <v>3</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H6" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="3">
         <v>389</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+      <c r="A7" s="26">
         <v>4</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H7" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="3">
         <v>390</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+      <c r="A8" s="26">
         <v>5</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H8" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H8" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="3">
         <v>391</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="26">
         <v>6</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H9" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H9" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="3">
         <v>392</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+      <c r="A10" s="26">
         <v>7</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H10" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H10" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="3">
         <v>393</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+      <c r="A11" s="26">
         <v>8</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H11" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H11" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J11" s="3">
         <v>394</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="32">
+      <c r="A12" s="26">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H12" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H12" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J12" s="3">
         <v>395</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+      <c r="A13" s="26">
         <v>10</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H13" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H13" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="3">
         <v>396</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="26">
         <v>11</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="3">
         <v>397</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+      <c r="A15" s="26">
         <v>12</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H15" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="3">
         <v>398</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="26">
         <v>13</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H16" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="3">
         <v>399</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="A17" s="26">
         <v>14</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H17" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="3">
         <v>400</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
+      <c r="A18" s="26">
         <v>15</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H18" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H18" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J18" s="3">
         <v>401</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
+      <c r="A19" s="26">
         <v>16</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H19" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H19" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J19" s="3">
         <v>402</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="26">
         <v>17</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H20" s="26" t="e">
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H20" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
+      <c r="A21" s="26">
         <v>18</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H21" s="26" t="e">
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H21" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="32">
+      <c r="A22" s="26">
         <v>19</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J22" s="9" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H22" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="K22" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="32">
+      <c r="A23" s="26">
         <v>20</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H23" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J23" s="9">
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H23" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J23" s="8">
         <v>1</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="K23" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="32">
+      <c r="A24" s="26">
         <v>21</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H24" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J24" s="9">
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H24" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J24" s="8">
         <v>2</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="K24" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
+      <c r="A25" s="26">
         <v>22</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H25" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J25" s="9">
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H25" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J25" s="8">
         <v>3</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="32">
+      <c r="A26" s="26">
         <v>23</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H26" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J26" s="9">
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H26" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J26" s="8">
         <v>4</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="32">
+      <c r="A27" s="26">
         <v>24</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H27" s="26" t="e">
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H27" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="32">
+      <c r="A28" s="26">
         <v>25</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H28" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H28" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="32">
+      <c r="A29" s="26">
         <v>26</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H29" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H29" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
+      <c r="A30" s="26">
         <v>27</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H30" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H30" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="32">
+      <c r="A31" s="26">
         <v>28</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H31" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H31" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="32">
+      <c r="A32" s="26">
         <v>29</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H32" s="26" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H32" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="32">
+      <c r="A33" s="26">
         <v>30</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H33" s="26" t="e">
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H33" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="32">
+      <c r="A34" s="26">
         <v>31</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H34" s="26" t="e">
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H34" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="32">
+      <c r="A35" s="26">
         <v>32</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H35" s="26" t="e">
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H35" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="32">
+      <c r="A36" s="26">
         <v>33</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H36" s="26" t="e">
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H36" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="32">
+      <c r="A37" s="26">
         <v>34</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F37" s="27"/>
-      <c r="G37" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H37" s="26" t="e">
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F37" s="21"/>
+      <c r="G37" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H37" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="32">
+      <c r="A38" s="26">
         <v>35</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H38" s="26" t="e">
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="G38" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H38" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="32">
+      <c r="A39" s="26">
         <v>36</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H39" s="26" t="e">
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H39" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="32">
+      <c r="A40" s="26">
         <v>37</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F40" s="27"/>
-      <c r="G40" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="26" t="e">
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H40" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="32">
+      <c r="A41" s="26">
         <v>38</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F41" s="27"/>
-      <c r="G41" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H41" s="26" t="e">
+      <c r="B41" s="21"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H41" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="32">
+      <c r="A42" s="26">
         <v>39</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F42" s="27"/>
-      <c r="G42" s="26" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H42" s="26" t="e">
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H42" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="32">
+      <c r="A43" s="26">
         <v>40</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F43" s="27"/>
-      <c r="G43" s="26" t="e">
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20" t="e">
         <f>VLOOKUP(F43,J43:L58,2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H43" s="26" t="e">
+      <c r="H43" s="20" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="32">
+      <c r="A44" s="26">
         <v>41</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="25" t="e">
+      <c r="B44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="19" t="e">
         <f t="shared" ref="E44:E53" si="3">VLOOKUP(D44,J63:K66,2)</f>
         <v>#N/A</v>
       </c>
-      <c r="F44" s="27"/>
-      <c r="G44" s="26" t="e">
+      <c r="F44" s="21"/>
+      <c r="G44" s="20" t="e">
         <f t="shared" ref="G44:G53" si="4">VLOOKUP(F44,J44:L59,2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H44" s="26" t="e">
+      <c r="H44" s="20" t="e">
         <f t="shared" ref="H44:H53" si="5">VLOOKUP(F44,J44:L59,3)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="32">
+      <c r="A45" s="26">
         <v>42</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="25" t="e">
+      <c r="B45" s="21"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F45" s="27"/>
-      <c r="G45" s="26" t="e">
+      <c r="F45" s="21"/>
+      <c r="G45" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H45" s="26" t="e">
+      <c r="H45" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="32">
+      <c r="A46" s="26">
         <v>43</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="25" t="e">
+      <c r="B46" s="21"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F46" s="27"/>
-      <c r="G46" s="26" t="e">
+      <c r="F46" s="21"/>
+      <c r="G46" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H46" s="26" t="e">
+      <c r="H46" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="32">
+      <c r="A47" s="26">
         <v>44</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="25" t="e">
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="26" t="e">
+      <c r="F47" s="21"/>
+      <c r="G47" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H47" s="26" t="e">
+      <c r="H47" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="32">
+      <c r="A48" s="26">
         <v>45</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="25" t="e">
+      <c r="B48" s="21"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="26" t="e">
+      <c r="F48" s="21"/>
+      <c r="G48" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H48" s="26" t="e">
+      <c r="H48" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="32">
+      <c r="A49" s="26">
         <v>46</v>
       </c>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="25" t="e">
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F49" s="27"/>
-      <c r="G49" s="26" t="e">
+      <c r="F49" s="21"/>
+      <c r="G49" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H49" s="26" t="e">
+      <c r="H49" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="32">
+      <c r="A50" s="26">
         <v>47</v>
       </c>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="25" t="e">
+      <c r="B50" s="21"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F50" s="27"/>
-      <c r="G50" s="26" t="e">
+      <c r="F50" s="21"/>
+      <c r="G50" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H50" s="26" t="e">
+      <c r="H50" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="32">
+      <c r="A51" s="26">
         <v>48</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="25" t="e">
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F51" s="27"/>
-      <c r="G51" s="26" t="e">
+      <c r="F51" s="21"/>
+      <c r="G51" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H51" s="26" t="e">
+      <c r="H51" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="32">
+      <c r="A52" s="26">
         <v>49</v>
       </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="25" t="e">
+      <c r="B52" s="21"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F52" s="27"/>
-      <c r="G52" s="26" t="e">
+      <c r="F52" s="21"/>
+      <c r="G52" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H52" s="26" t="e">
+      <c r="H52" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="32">
+      <c r="A53" s="26">
         <v>50</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="25" t="e">
+      <c r="B53" s="21"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="19" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F53" s="27"/>
-      <c r="G53" s="26" t="e">
+      <c r="F53" s="21"/>
+      <c r="G53" s="20" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="H53" s="26" t="e">
+      <c r="H53" s="20" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
+      <c r="C54" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <sheetProtection password="CE28" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="4">
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="A1:C2"/>
+    <mergeCell ref="F1:H2"/>
+    <mergeCell ref="D1:E2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F4:F53">

</xml_diff>

<commit_message>
Commit new employee_upload template
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/general/employee_upload.xlsx
+++ b/file/template/pusdiklat/general/employee_upload.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="8595" windowHeight="1875"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$F$4</definedName>
     <definedName name="NAMA_UNIT">Sheet2!$A$1:$A$13</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -947,7 +947,7 @@
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,18 +1046,18 @@
         <v>4</v>
       </c>
       <c r="E4" s="19" t="str">
-        <f>VLOOKUP(D4,J23:K26,2)</f>
+        <f>VLOOKUP(D4,$J$23:$K$26,2)</f>
         <v>PRANATA KOMPUTER</v>
       </c>
       <c r="F4" s="21">
         <v>389</v>
       </c>
       <c r="G4" s="20" t="str">
-        <f>VLOOKUP(F4,J4:L19,2)</f>
+        <f>VLOOKUP(F4,$J$4:$L$19,2)</f>
         <v>1213010100</v>
       </c>
       <c r="H4" s="20" t="str">
-        <f>VLOOKUP(F4,J4:L19,3)</f>
+        <f>VLOOKUP(F4,$J$4:$L$19,3)</f>
         <v>Subbagian Tata Usaha, Kepegawaian Dan Hubungan Mas...</v>
       </c>
       <c r="J4" s="3">
@@ -1076,18 +1076,18 @@
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="19" t="e">
-        <f t="shared" ref="E5:E43" si="0">VLOOKUP(D5,J24:K27,2)</f>
+        <f t="shared" ref="E5:E53" si="0">VLOOKUP(D5,$J$23:$K$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="20" t="e">
-        <f t="shared" ref="G5:G42" si="1">VLOOKUP(F5,J5:L20,2)</f>
+        <f t="shared" ref="G5:G53" si="1">VLOOKUP(F5,$J$4:$L$19,2)</f>
         <v>#N/A</v>
       </c>
       <c r="H5" s="20" t="e">
-        <f t="shared" ref="H5:H43" si="2">VLOOKUP(F5,J5:L20,3)</f>
+        <f t="shared" ref="H5:H53" si="2">VLOOKUP(F5,$J$4:$L$19,3)</f>
         <v>#N/A</v>
       </c>
       <c r="J5" s="3">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="21"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
-      <c r="D9" s="21"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
-      <c r="D10" s="21"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="21"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="21"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="21"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="21"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
-      <c r="D15" s="21"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="21"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="21"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
-      <c r="D22" s="21"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
-      <c r="D24" s="21"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1812,7 +1812,7 @@
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
-      <c r="D32" s="21"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="22"/>
-      <c r="D34" s="21"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
-      <c r="D37" s="21"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="21"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
-      <c r="D39" s="21"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="22"/>
-      <c r="D40" s="21"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="22"/>
-      <c r="D41" s="21"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
-      <c r="D42" s="21"/>
+      <c r="D42" s="18"/>
       <c r="E42" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
@@ -2044,14 +2044,14 @@
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
-      <c r="D43" s="21"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="20" t="e">
-        <f>VLOOKUP(F43,J43:L58,2)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H43" s="20" t="e">
@@ -2065,18 +2065,18 @@
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="22"/>
-      <c r="D44" s="21"/>
+      <c r="D44" s="18"/>
       <c r="E44" s="19" t="e">
-        <f t="shared" ref="E44:E53" si="3">VLOOKUP(D44,J63:K66,2)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="20" t="e">
-        <f t="shared" ref="G44:G53" si="4">VLOOKUP(F44,J44:L59,2)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H44" s="20" t="e">
-        <f t="shared" ref="H44:H53" si="5">VLOOKUP(F44,J44:L59,3)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2086,18 +2086,18 @@
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="22"/>
-      <c r="D45" s="21"/>
+      <c r="D45" s="18"/>
       <c r="E45" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H45" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2107,18 +2107,18 @@
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="22"/>
-      <c r="D46" s="21"/>
+      <c r="D46" s="18"/>
       <c r="E46" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H46" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2128,18 +2128,18 @@
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="22"/>
-      <c r="D47" s="21"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H47" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2149,18 +2149,18 @@
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="22"/>
-      <c r="D48" s="21"/>
+      <c r="D48" s="18"/>
       <c r="E48" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H48" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2170,18 +2170,18 @@
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="22"/>
-      <c r="D49" s="21"/>
+      <c r="D49" s="18"/>
       <c r="E49" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H49" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2191,18 +2191,18 @@
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="22"/>
-      <c r="D50" s="21"/>
+      <c r="D50" s="18"/>
       <c r="E50" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H50" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2212,18 +2212,18 @@
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="22"/>
-      <c r="D51" s="21"/>
+      <c r="D51" s="18"/>
       <c r="E51" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H51" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2233,18 +2233,18 @@
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="22"/>
-      <c r="D52" s="21"/>
+      <c r="D52" s="18"/>
       <c r="E52" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H52" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2254,18 +2254,18 @@
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="22"/>
-      <c r="D53" s="21"/>
+      <c r="D53" s="18"/>
       <c r="E53" s="19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="20" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="H53" s="20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
       <formula1>$J$4:$J$19</formula1>
     </dataValidation>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Data Tidak Valid" error="Lihat Kode Organisasi" sqref="G4:H53"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D53">
       <formula1>$J$23:$J$26</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Upload Person bisa 100
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/general/employee_upload.xlsx
+++ b/file/template/pusdiklat/general/employee_upload.xlsx
@@ -264,7 +264,7 @@
     <t>NAMA JABATAN</t>
   </si>
   <si>
-    <t>STOP HERE</t>
+    <t>BERHENTI DISINI</t>
   </si>
 </sst>
 </file>
@@ -944,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,16 +1078,16 @@
       <c r="C5" s="22"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="e">
-        <f t="shared" ref="E5:E53" si="0">VLOOKUP(D5,$J$23:$K$26,2)</f>
+        <f t="shared" ref="E5:E51" si="0">VLOOKUP(D5,$J$23:$K$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="20" t="e">
-        <f t="shared" ref="G5:G53" si="1">VLOOKUP(F5,$J$4:$L$19,2)</f>
+        <f t="shared" ref="G5:G52" si="1">VLOOKUP(F5,$J$4:$L$19,2)</f>
         <v>#N/A</v>
       </c>
       <c r="H5" s="20" t="e">
-        <f t="shared" ref="H5:H53" si="2">VLOOKUP(F5,$J$4:$L$19,3)</f>
+        <f t="shared" ref="H5:H52" si="2">VLOOKUP(F5,$J$4:$L$19,3)</f>
         <v>#N/A</v>
       </c>
       <c r="J5" s="3">
@@ -2235,7 +2235,7 @@
       <c r="C52" s="22"/>
       <c r="D52" s="18"/>
       <c r="E52" s="19" t="e">
-        <f t="shared" si="0"/>
+        <f>VLOOKUP(D52,$J$23:$K$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="F52" s="21"/>
@@ -2256,32 +2256,1082 @@
       <c r="C53" s="22"/>
       <c r="D53" s="18"/>
       <c r="E53" s="19" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E53:E103" si="3">VLOOKUP(D53,$J$23:$K$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="20" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G53:G103" si="4">VLOOKUP(F53,$J$4:$L$19,2)</f>
         <v>#N/A</v>
       </c>
       <c r="H53" s="20" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H53:H103" si="5">VLOOKUP(F53,$J$4:$L$19,3)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23" t="s">
+      <c r="A54" s="26">
+        <v>51</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F54" s="21"/>
+      <c r="G54" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H54" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="26">
+        <v>52</v>
+      </c>
+      <c r="B55" s="21"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H55" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="26">
+        <v>53</v>
+      </c>
+      <c r="B56" s="21"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F56" s="21"/>
+      <c r="G56" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H56" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="26">
+        <v>54</v>
+      </c>
+      <c r="B57" s="21"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H57" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="26">
+        <v>55</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H58" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="26">
+        <v>56</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F59" s="21"/>
+      <c r="G59" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H59" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="26">
+        <v>57</v>
+      </c>
+      <c r="B60" s="21"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F60" s="21"/>
+      <c r="G60" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H60" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="26">
+        <v>58</v>
+      </c>
+      <c r="B61" s="21"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F61" s="21"/>
+      <c r="G61" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H61" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="26">
+        <v>59</v>
+      </c>
+      <c r="B62" s="21"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F62" s="21"/>
+      <c r="G62" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H62" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="26">
+        <v>60</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F63" s="21"/>
+      <c r="G63" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H63" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="26">
+        <v>61</v>
+      </c>
+      <c r="B64" s="21"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F64" s="21"/>
+      <c r="G64" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H64" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="26">
+        <v>62</v>
+      </c>
+      <c r="B65" s="21"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F65" s="21"/>
+      <c r="G65" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H65" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="26">
+        <v>63</v>
+      </c>
+      <c r="B66" s="21"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F66" s="21"/>
+      <c r="G66" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H66" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="26">
         <v>64</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="B67" s="21"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F67" s="21"/>
+      <c r="G67" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H67" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="26">
+        <v>65</v>
+      </c>
+      <c r="B68" s="21"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F68" s="21"/>
+      <c r="G68" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H68" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="26">
+        <v>66</v>
+      </c>
+      <c r="B69" s="21"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F69" s="21"/>
+      <c r="G69" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H69" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="26">
+        <v>67</v>
+      </c>
+      <c r="B70" s="21"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F70" s="21"/>
+      <c r="G70" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H70" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="26">
+        <v>68</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F71" s="21"/>
+      <c r="G71" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H71" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="26">
+        <v>69</v>
+      </c>
+      <c r="B72" s="21"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F72" s="21"/>
+      <c r="G72" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H72" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="26">
+        <v>70</v>
+      </c>
+      <c r="B73" s="21"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F73" s="21"/>
+      <c r="G73" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H73" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="26">
+        <v>71</v>
+      </c>
+      <c r="B74" s="21"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F74" s="21"/>
+      <c r="G74" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H74" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="26">
+        <v>72</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F75" s="21"/>
+      <c r="G75" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H75" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="26">
+        <v>73</v>
+      </c>
+      <c r="B76" s="21"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F76" s="21"/>
+      <c r="G76" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H76" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="26">
+        <v>74</v>
+      </c>
+      <c r="B77" s="21"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F77" s="21"/>
+      <c r="G77" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H77" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="26">
+        <v>75</v>
+      </c>
+      <c r="B78" s="21"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F78" s="21"/>
+      <c r="G78" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H78" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="26">
+        <v>76</v>
+      </c>
+      <c r="B79" s="21"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H79" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="26">
+        <v>77</v>
+      </c>
+      <c r="B80" s="21"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F80" s="21"/>
+      <c r="G80" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H80" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="26">
+        <v>78</v>
+      </c>
+      <c r="B81" s="21"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F81" s="21"/>
+      <c r="G81" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H81" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="26">
+        <v>79</v>
+      </c>
+      <c r="B82" s="21"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F82" s="21"/>
+      <c r="G82" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H82" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="26">
+        <v>80</v>
+      </c>
+      <c r="B83" s="21"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F83" s="21"/>
+      <c r="G83" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H83" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="26">
+        <v>81</v>
+      </c>
+      <c r="B84" s="21"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F84" s="21"/>
+      <c r="G84" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H84" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="26">
+        <v>82</v>
+      </c>
+      <c r="B85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F85" s="21"/>
+      <c r="G85" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H85" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>83</v>
+      </c>
+      <c r="B86" s="21"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F86" s="21"/>
+      <c r="G86" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H86" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="26">
+        <v>84</v>
+      </c>
+      <c r="B87" s="21"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F87" s="21"/>
+      <c r="G87" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H87" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="26">
+        <v>85</v>
+      </c>
+      <c r="B88" s="21"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F88" s="21"/>
+      <c r="G88" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H88" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="26">
+        <v>86</v>
+      </c>
+      <c r="B89" s="21"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F89" s="21"/>
+      <c r="G89" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H89" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="26">
+        <v>87</v>
+      </c>
+      <c r="B90" s="21"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F90" s="21"/>
+      <c r="G90" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H90" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="26">
+        <v>88</v>
+      </c>
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F91" s="21"/>
+      <c r="G91" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H91" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="26">
+        <v>89</v>
+      </c>
+      <c r="B92" s="21"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F92" s="21"/>
+      <c r="G92" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H92" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="26">
+        <v>90</v>
+      </c>
+      <c r="B93" s="21"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F93" s="21"/>
+      <c r="G93" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H93" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="26">
+        <v>91</v>
+      </c>
+      <c r="B94" s="21"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F94" s="21"/>
+      <c r="G94" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H94" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="26">
+        <v>92</v>
+      </c>
+      <c r="B95" s="21"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F95" s="21"/>
+      <c r="G95" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H95" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="26">
+        <v>93</v>
+      </c>
+      <c r="B96" s="21"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F96" s="21"/>
+      <c r="G96" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H96" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="26">
+        <v>94</v>
+      </c>
+      <c r="B97" s="21"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F97" s="21"/>
+      <c r="G97" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H97" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="26">
+        <v>95</v>
+      </c>
+      <c r="B98" s="21"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F98" s="21"/>
+      <c r="G98" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H98" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="26">
+        <v>96</v>
+      </c>
+      <c r="B99" s="21"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F99" s="21"/>
+      <c r="G99" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H99" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="26">
+        <v>97</v>
+      </c>
+      <c r="B100" s="21"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F100" s="21"/>
+      <c r="G100" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H100" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="26">
+        <v>98</v>
+      </c>
+      <c r="B101" s="21"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F101" s="21"/>
+      <c r="G101" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H101" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="26">
+        <v>99</v>
+      </c>
+      <c r="B102" s="21"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F102" s="21"/>
+      <c r="G102" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H102" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="26">
+        <v>100</v>
+      </c>
+      <c r="B103" s="21"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="19" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F103" s="21"/>
+      <c r="G103" s="20" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H103" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="23"/>
+      <c r="B104" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
     </row>
   </sheetData>
   <sheetProtection password="CE28" sheet="1" objects="1" scenarios="1"/>
@@ -2292,11 +3342,11 @@
     <mergeCell ref="D1:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F4:F53">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F4:F103">
       <formula1>$J$4:$J$19</formula1>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Data Tidak Valid" error="Lihat Kode Organisasi" sqref="G4:H53"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D53">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Data Tidak Valid" error="Lihat Kode Organisasi" sqref="G4:H103"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D103">
       <formula1>$J$23:$J$26</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>